<commit_message>
Changed layout and added Video feature
New improved layout
Added feature where a video of the plot is generated
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/cmtmd_leeds_ac_uk/Documents/PhD project infomation/Data/Code/MATLAB/Practise/Design space code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/cmtmd_leeds_ac_uk/Documents/PhD project infomation/Data/Code/MATLAB/Practise/Design space code/DesignSpace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{5126B65A-895C-4225-9596-EDBA89B1D149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{477295C7-C201-4B88-9A36-C528129621AB}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{5126B65A-895C-4225-9596-EDBA89B1D149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39D5B850-1761-478D-AE38-F775AD034147}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E74FF3C7-3431-46FA-8731-11E5BAF30EB7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E74FF3C7-3431-46FA-8731-11E5BAF30EB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,19 @@
     <t>Results</t>
   </si>
   <si>
-    <t>Variable 1</t>
-  </si>
-  <si>
-    <t>Variable 2</t>
-  </si>
-  <si>
     <t>Variable 4</t>
   </si>
   <si>
-    <t>Variable 3</t>
+    <t>Variable 5</t>
   </si>
   <si>
-    <t>Variable 5</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,19 +416,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>

</xml_diff>